<commit_message>
template docx and xlsx files changes
</commit_message>
<xml_diff>
--- a/templates/cpr1000/bdsd_check_list.xlsx
+++ b/templates/cpr1000/bdsd_check_list.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\doc-server\templates\cpr1000\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="12045"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">SAMA图纸检查内容表!$A$1:$J$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">SAMA图纸检查内容表!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -510,10 +515,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${project}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>${t}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -531,12 +532,16 @@
   </si>
   <si>
     <t>${r_b}</t>
+  </si>
+  <si>
+    <t>${unit}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -791,13 +796,94 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,13 +893,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -822,94 +914,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -919,6 +924,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -965,7 +978,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -997,9 +1010,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1031,6 +1045,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1206,896 +1221,938 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="7.125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="10.25" style="41" customWidth="1"/>
-    <col min="4" max="4" width="10" style="39" customWidth="1"/>
-    <col min="5" max="5" width="22.875" style="39" customWidth="1"/>
-    <col min="6" max="6" width="36.375" style="39" customWidth="1"/>
-    <col min="7" max="7" width="7.625" style="39" customWidth="1"/>
-    <col min="8" max="8" width="11.875" style="39" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="12.625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="7.125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10" style="13" customWidth="1"/>
+    <col min="5" max="5" width="22.875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="36.375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="7.625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="11.875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="36"/>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="40"/>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="24.95" customHeight="1">
+      <c r="A4" s="34"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="24.95" customHeight="1">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="9" t="s">
+      <c r="I4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="8" customFormat="1" ht="24.95" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1">
+      <c r="A6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1">
+      <c r="A7" s="27"/>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="33" customHeight="1">
+      <c r="A8" s="27"/>
+      <c r="B8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="18" customHeight="1">
+      <c r="A9" s="27"/>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="24" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A5" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1">
-      <c r="A6" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="31"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="31"/>
-    </row>
-    <row r="8" spans="1:10" ht="33" customHeight="1">
-      <c r="A8" s="32"/>
-      <c r="B8" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="31"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1">
-      <c r="A9" s="32"/>
-      <c r="B9" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="28" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="31"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="28" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="31"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="31"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="18" customHeight="1">
-      <c r="A12" s="32"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="28" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="31"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="26" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="31"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1">
-      <c r="A14" s="32"/>
-      <c r="B14" s="26" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="28" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="31"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="28" t="s">
+      <c r="E15" s="17"/>
+      <c r="F15" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="31"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A16" s="32"/>
-      <c r="B16" s="26" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="28" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="31"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="26" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="28" t="s">
+      <c r="E17" s="17"/>
+      <c r="F17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="31"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="27" customHeight="1">
-      <c r="A18" s="32"/>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="27"/>
+      <c r="B18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="19"/>
+      <c r="D18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="28" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="31"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="26" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28" t="s">
+      <c r="C19" s="19"/>
+      <c r="D19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="28" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="31"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="18" customHeight="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="26" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="28" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="31"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="28" t="s">
+      <c r="E21" s="17"/>
+      <c r="F21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="31"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A22" s="35"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="28" t="s">
+      <c r="E22" s="17"/>
+      <c r="F22" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="31"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A23" s="35"/>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="28" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="31"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A24" s="35"/>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="28" t="s">
+      <c r="E24" s="17"/>
+      <c r="F24" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="31"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="34.5" customHeight="1">
-      <c r="A25" s="35"/>
-      <c r="B25" s="26" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="28" t="s">
+      <c r="E25" s="17"/>
+      <c r="F25" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="31"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A26" s="35"/>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="28" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="31"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A27" s="35"/>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="28" t="s">
+      <c r="E27" s="17"/>
+      <c r="F27" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="31"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" ht="22.5" customHeight="1">
-      <c r="A28" s="35"/>
-      <c r="B28" s="26" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="28" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="28" t="s">
+      <c r="E28" s="17"/>
+      <c r="F28" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="31"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" ht="18" customHeight="1">
-      <c r="A29" s="35"/>
-      <c r="B29" s="26" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="28" t="s">
+      <c r="E29" s="17"/>
+      <c r="F29" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="31"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A30" s="35"/>
-      <c r="B30" s="26" t="s">
+      <c r="A30" s="21"/>
+      <c r="B30" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="28" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="28" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J30" s="31"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
-      <c r="A31" s="35"/>
-      <c r="B31" s="26" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="28" t="s">
+      <c r="E31" s="17"/>
+      <c r="F31" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J31" s="31"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A32" s="35"/>
-      <c r="B32" s="26" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="28" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="28" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J32" s="31"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J32" s="10"/>
     </row>
     <row r="33" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A33" s="35"/>
-      <c r="B33" s="26" t="s">
+      <c r="A33" s="21"/>
+      <c r="B33" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="28" t="s">
+      <c r="C33" s="19"/>
+      <c r="D33" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="28" t="s">
+      <c r="E33" s="17"/>
+      <c r="F33" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="G33" s="30"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="31"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="10"/>
     </row>
     <row r="34" spans="1:10" ht="18" customHeight="1">
-      <c r="A34" s="35"/>
-      <c r="B34" s="26" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="28" t="s">
+      <c r="C34" s="19"/>
+      <c r="D34" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="28" t="s">
+      <c r="E34" s="17"/>
+      <c r="F34" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="G34" s="30"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="31"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="10"/>
     </row>
     <row r="35" spans="1:10" ht="18" customHeight="1">
-      <c r="A35" s="35"/>
-      <c r="B35" s="26" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="28" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="28" t="s">
+      <c r="E35" s="17"/>
+      <c r="F35" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J35" s="31"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="10"/>
     </row>
     <row r="36" spans="1:10" ht="30.75" customHeight="1">
-      <c r="A36" s="35"/>
-      <c r="B36" s="26" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28" t="s">
+      <c r="C36" s="19"/>
+      <c r="D36" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="28" t="s">
+      <c r="E36" s="17"/>
+      <c r="F36" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J36" s="31"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A37" s="35"/>
-      <c r="B37" s="26" t="s">
+      <c r="A37" s="21"/>
+      <c r="B37" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="28" t="s">
+      <c r="C37" s="19"/>
+      <c r="D37" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="28" t="s">
+      <c r="E37" s="17"/>
+      <c r="F37" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="31"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" ht="18" customHeight="1">
-      <c r="A38" s="35"/>
-      <c r="B38" s="26" t="s">
+      <c r="A38" s="21"/>
+      <c r="B38" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="28" t="s">
+      <c r="E38" s="17"/>
+      <c r="F38" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J38" s="31"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J38" s="10"/>
     </row>
     <row r="39" spans="1:10" ht="33.75" customHeight="1">
-      <c r="A39" s="35"/>
-      <c r="B39" s="26" t="s">
+      <c r="A39" s="21"/>
+      <c r="B39" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="28" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="28" t="s">
+      <c r="E39" s="17"/>
+      <c r="F39" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J39" s="31"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A40" s="35"/>
-      <c r="B40" s="26" t="s">
+      <c r="A40" s="21"/>
+      <c r="B40" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="28" t="s">
+      <c r="C40" s="19"/>
+      <c r="D40" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="28" t="s">
+      <c r="E40" s="17"/>
+      <c r="F40" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="G40" s="30"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" s="31"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="10"/>
     </row>
     <row r="41" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A41" s="36"/>
-      <c r="B41" s="26" t="s">
+      <c r="A41" s="22"/>
+      <c r="B41" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28" t="s">
+      <c r="C41" s="19"/>
+      <c r="D41" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="28" t="s">
+      <c r="E41" s="17"/>
+      <c r="F41" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="G41" s="30"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="J41" s="31"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="10"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="F43" s="40"/>
+      <c r="C43" s="12"/>
+      <c r="F43" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="A6:A20"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="A21:A41"/>
+    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:H27"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="D28:E28"/>
@@ -2108,65 +2165,23 @@
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="A21:A41"/>
-    <mergeCell ref="C21:C28"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="A6:A20"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:H41"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>